<commit_message>
cronograma: experimento como expansor/ranker
</commit_message>
<xml_diff>
--- a/docs/schedule/cronograma.xlsx
+++ b/docs/schedule/cronograma.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0FF740-6684-49A3-871A-0848BCE5E433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9BA698B-CB5A-4B7D-9DB8-3B31316A9368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CronogramaDeProjeto" sheetId="11" r:id="rId1"/>
@@ -282,9 +282,6 @@
     <t>Realizar experimentos: indexador como pipeline de busca</t>
   </si>
   <si>
-    <t>Realizar experimentos: indexador como ranker</t>
-  </si>
-  <si>
     <t>Preparar apresentação final</t>
   </si>
   <si>
@@ -319,6 +316,9 @@
   </si>
   <si>
     <t>Construção do Dataset de Avaliação de Busca (Juris-TCU)</t>
+  </si>
+  <si>
+    <t>Realizar experimentos: indexador como expansor/ranker</t>
   </si>
 </sst>
 </file>
@@ -326,13 +326,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="7">
-    <numFmt numFmtId="42" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="d/m/yy;@"/>
-    <numFmt numFmtId="166" formatCode="d\-mmm\-yyyy"/>
-    <numFmt numFmtId="167" formatCode="d"/>
-    <numFmt numFmtId="168" formatCode="ddd\,\ dd/mm/yyyy"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="d/m/yy;@"/>
+    <numFmt numFmtId="168" formatCode="d\-mmm\-yyyy"/>
+    <numFmt numFmtId="169" formatCode="d"/>
+    <numFmt numFmtId="170" formatCode="ddd\,\ dd/mm/yyyy"/>
   </numFmts>
   <fonts count="38" x14ac:knownFonts="1">
     <font>
@@ -1109,10 +1109,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="3">
+    <xf numFmtId="170" fontId="6" fillId="0" borderId="3">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="2" applyFill="0">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="2" applyFill="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyFill="0">
@@ -1122,9 +1122,9 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1283,37 +1283,37 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="2" xfId="10" applyFill="1">
+    <xf numFmtId="167" fontId="6" fillId="2" borderId="2" xfId="10" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="3" borderId="2" xfId="10" applyFill="1">
+    <xf numFmtId="167" fontId="6" fillId="3" borderId="2" xfId="10" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="8" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="8" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="41" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="8" fillId="41" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="41" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1353,10 +1353,10 @@
     <xf numFmtId="0" fontId="35" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="36" fillId="42" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="36" fillId="42" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="19" fillId="42" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="19" fillId="42" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1369,7 +1369,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="4" borderId="2" xfId="10" applyFill="1">
+    <xf numFmtId="167" fontId="6" fillId="4" borderId="2" xfId="10" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="12" applyFill="1">
@@ -1384,7 +1384,7 @@
     <xf numFmtId="0" fontId="6" fillId="43" borderId="2" xfId="12" applyFill="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="43" borderId="2" xfId="10" applyFill="1">
+    <xf numFmtId="167" fontId="6" fillId="43" borderId="2" xfId="10" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="43" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
@@ -1399,10 +1399,10 @@
     <xf numFmtId="9" fontId="3" fillId="44" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="44" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="44" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="44" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="44" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="45" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1414,10 +1414,10 @@
     <xf numFmtId="9" fontId="3" fillId="45" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="45" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="45" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="45" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="45" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5" applyAlignment="1"/>
@@ -1430,7 +1430,7 @@
     <xf numFmtId="9" fontId="3" fillId="3" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="3" borderId="17" xfId="10" applyFill="1" applyBorder="1">
+    <xf numFmtId="167" fontId="6" fillId="3" borderId="17" xfId="10" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="6" applyAlignment="1">
@@ -1444,19 +1444,19 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="168" fontId="19" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1">
+    <xf numFmtId="170" fontId="19" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2111,29 +2111,29 @@
   <dimension ref="A1:BD42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M24" sqref="M24"/>
+      <pane ySplit="7" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="31" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="31" customWidth="1"/>
     <col min="2" max="2" width="61" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" customWidth="1"/>
-    <col min="7" max="7" width="2.77734375" customWidth="1"/>
-    <col min="8" max="8" width="6.21875" hidden="1" customWidth="1"/>
-    <col min="9" max="51" width="2.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="2.7109375" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" hidden="1" customWidth="1"/>
+    <col min="9" max="51" width="2.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" ht="26.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:56" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="92" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C1" s="92"/>
       <c r="D1" s="1"/>
@@ -2141,10 +2141,10 @@
       <c r="F1" s="20"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:56" ht="24.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:56" ht="24.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="32"/>
       <c r="B2" s="92" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C2" s="92"/>
       <c r="D2" s="1"/>
@@ -2152,7 +2152,7 @@
       <c r="F2" s="20"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
         <v>1</v>
       </c>
@@ -2160,14 +2160,14 @@
         <v>51</v>
       </c>
       <c r="C3" s="98" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I3" s="43" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="BD3" s="100"/>
     </row>
-    <row r="4" spans="1:56" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:56" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>2</v>
       </c>
@@ -2181,7 +2181,7 @@
       </c>
       <c r="F4" s="106"/>
     </row>
-    <row r="5" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
         <v>3</v>
       </c>
@@ -2244,7 +2244,7 @@
       <c r="AX5" s="104"/>
       <c r="AY5" s="54"/>
     </row>
-    <row r="6" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
         <v>4</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>45106</v>
       </c>
     </row>
-    <row r="7" spans="1:56" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:56" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="32" t="s">
         <v>5</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>q</v>
       </c>
     </row>
-    <row r="8" spans="1:56" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:56" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="31" t="s">
         <v>6</v>
       </c>
@@ -2677,7 +2677,7 @@
       <c r="AX8" s="18"/>
       <c r="AY8" s="18"/>
     </row>
-    <row r="9" spans="1:56" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:56" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="32" t="s">
         <v>7</v>
       </c>
@@ -2737,7 +2737,7 @@
       <c r="AX9" s="18"/>
       <c r="AY9" s="57"/>
     </row>
-    <row r="10" spans="1:56" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:56" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="32" t="s">
         <v>8</v>
       </c>
@@ -2806,7 +2806,7 @@
       <c r="AX10" s="18"/>
       <c r="AY10" s="57"/>
     </row>
-    <row r="11" spans="1:56" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:56" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="32" t="s">
         <v>9</v>
       </c>
@@ -2874,7 +2874,7 @@
       <c r="AX11" s="18"/>
       <c r="AY11" s="57"/>
     </row>
-    <row r="12" spans="1:56" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:56" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="31"/>
       <c r="B12" s="40" t="s">
         <v>37</v>
@@ -2941,7 +2941,7 @@
       <c r="AY12" s="57"/>
       <c r="BD12" s="99"/>
     </row>
-    <row r="13" spans="1:56" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:56" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="31"/>
       <c r="B13" s="40" t="s">
         <v>38</v>
@@ -3007,12 +3007,12 @@
       <c r="AX13" s="18"/>
       <c r="AY13" s="57"/>
     </row>
-    <row r="14" spans="1:56" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:56" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="32" t="s">
         <v>55</v>
       </c>
       <c r="B14" s="82" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C14" s="83"/>
       <c r="D14" s="84"/>
@@ -3067,12 +3067,12 @@
       <c r="AX14" s="18"/>
       <c r="AY14" s="57"/>
     </row>
-    <row r="15" spans="1:56" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:56" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="32" t="s">
         <v>55</v>
       </c>
       <c r="B15" s="74" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C15" s="39" t="s">
         <v>39</v>
@@ -3135,7 +3135,7 @@
       <c r="AX15" s="18"/>
       <c r="AY15" s="57"/>
     </row>
-    <row r="16" spans="1:56" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:56" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="32" t="s">
         <v>55</v>
       </c>
@@ -3203,7 +3203,7 @@
       <c r="AX16" s="18"/>
       <c r="AY16" s="57"/>
     </row>
-    <row r="17" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="32" t="s">
         <v>55</v>
       </c>
@@ -3271,7 +3271,7 @@
       <c r="AX17" s="18"/>
       <c r="AY17" s="57"/>
     </row>
-    <row r="18" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="31"/>
       <c r="B18" s="74" t="s">
         <v>59</v>
@@ -3337,12 +3337,12 @@
       <c r="AX18" s="18"/>
       <c r="AY18" s="57"/>
     </row>
-    <row r="19" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="32" t="s">
         <v>55</v>
       </c>
       <c r="B19" s="76" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C19" s="39" t="s">
         <v>49</v>
@@ -3405,7 +3405,7 @@
       <c r="AX19" s="18"/>
       <c r="AY19" s="57"/>
     </row>
-    <row r="20" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="31"/>
       <c r="B20" s="76" t="s">
         <v>58</v>
@@ -3471,12 +3471,12 @@
       <c r="AX20" s="18"/>
       <c r="AY20" s="57"/>
     </row>
-    <row r="21" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="32" t="s">
         <v>55</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C21" s="37"/>
       <c r="D21" s="15"/>
@@ -3531,10 +3531,10 @@
       <c r="AX21" s="18"/>
       <c r="AY21" s="57"/>
     </row>
-    <row r="22" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="31"/>
       <c r="B22" s="41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C22" s="38" t="s">
         <v>50</v>
@@ -3597,7 +3597,7 @@
       <c r="AX22" s="18"/>
       <c r="AY22" s="57"/>
     </row>
-    <row r="23" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="31"/>
       <c r="B23" s="41" t="s">
         <v>41</v>
@@ -3663,7 +3663,7 @@
       <c r="AX23" s="18"/>
       <c r="AY23" s="57"/>
     </row>
-    <row r="24" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="31"/>
       <c r="B24" s="41" t="s">
         <v>61</v>
@@ -3729,7 +3729,7 @@
       <c r="AX24" s="18"/>
       <c r="AY24" s="57"/>
     </row>
-    <row r="25" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="31"/>
       <c r="B25" s="41" t="s">
         <v>52</v>
@@ -3795,12 +3795,12 @@
       <c r="AX25" s="18"/>
       <c r="AY25" s="57"/>
     </row>
-    <row r="26" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="32" t="s">
         <v>10</v>
       </c>
       <c r="B26" s="87" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C26" s="88"/>
       <c r="D26" s="89"/>
@@ -3855,7 +3855,7 @@
       <c r="AX26" s="18"/>
       <c r="AY26" s="57"/>
     </row>
-    <row r="27" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="32"/>
       <c r="B27" s="81" t="s">
         <v>63</v>
@@ -3921,7 +3921,7 @@
       <c r="AX27" s="18"/>
       <c r="AY27" s="57"/>
     </row>
-    <row r="28" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="31"/>
       <c r="B28" s="79" t="s">
         <v>64</v>
@@ -3987,7 +3987,7 @@
       <c r="AX28" s="18"/>
       <c r="AY28" s="57"/>
     </row>
-    <row r="29" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="32"/>
       <c r="B29" s="81" t="s">
         <v>65</v>
@@ -4053,7 +4053,7 @@
       <c r="AX29" s="18"/>
       <c r="AY29" s="57"/>
     </row>
-    <row r="30" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="31"/>
       <c r="B30" s="79" t="s">
         <v>40</v>
@@ -4119,7 +4119,7 @@
       <c r="AX30" s="18"/>
       <c r="AY30" s="57"/>
     </row>
-    <row r="31" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="32" t="s">
         <v>10</v>
       </c>
@@ -4179,7 +4179,7 @@
       <c r="AX31" s="18"/>
       <c r="AY31" s="57"/>
     </row>
-    <row r="32" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="32"/>
       <c r="B32" s="74" t="s">
         <v>63</v>
@@ -4245,7 +4245,7 @@
       <c r="AX32" s="18"/>
       <c r="AY32" s="57"/>
     </row>
-    <row r="33" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="31"/>
       <c r="B33" s="76" t="s">
         <v>64</v>
@@ -4311,10 +4311,10 @@
       <c r="AX33" s="18"/>
       <c r="AY33" s="57"/>
     </row>
-    <row r="34" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="31"/>
       <c r="B34" s="76" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="C34" s="39" t="s">
         <v>39</v>
@@ -4377,7 +4377,7 @@
       <c r="AX34" s="18"/>
       <c r="AY34" s="57"/>
     </row>
-    <row r="35" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="31" t="s">
         <v>11</v>
       </c>
@@ -4437,7 +4437,7 @@
       <c r="AX35" s="18"/>
       <c r="AY35" s="57"/>
     </row>
-    <row r="36" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="31"/>
       <c r="B36" s="41" t="s">
         <v>42</v>
@@ -4503,10 +4503,10 @@
       <c r="AX36" s="18"/>
       <c r="AY36" s="57"/>
     </row>
-    <row r="37" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="31"/>
       <c r="B37" s="93" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C37" s="94" t="s">
         <v>39</v>
@@ -4569,10 +4569,10 @@
       <c r="AX37" s="60"/>
       <c r="AY37" s="61"/>
     </row>
-    <row r="38" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="31"/>
       <c r="B38" s="93" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C38" s="94" t="s">
         <v>39</v>
@@ -4635,7 +4635,7 @@
       <c r="AX38" s="60"/>
       <c r="AY38" s="61"/>
     </row>
-    <row r="39" spans="1:51" s="65" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:51" s="65" customFormat="1" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="66" t="s">
         <v>12</v>
       </c>
@@ -4652,16 +4652,16 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:51" s="71" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:51" s="71" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="62"/>
       <c r="E40" s="72"/>
       <c r="G40" s="73"/>
     </row>
-    <row r="41" spans="1:51" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:51" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C41" s="8"/>
       <c r="F41" s="33"/>
     </row>
-    <row r="42" spans="1:51" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:51" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C42" s="9"/>
     </row>
   </sheetData>
@@ -4762,86 +4762,86 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="94.44140625" style="21" customWidth="1"/>
-    <col min="2" max="16384" width="9.21875" style="1"/>
+    <col min="1" max="1" width="94.42578125" style="21" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:2" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:2" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="22"/>
     </row>
-    <row r="3" spans="1:2" s="27" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="27" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="44" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="28"/>
     </row>
-    <row r="4" spans="1:2" s="24" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:2" s="24" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A4" s="25" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="26" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="21" customFormat="1" ht="205.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" s="21" customFormat="1" ht="205.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="24" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:2" s="24" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A8" s="25" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.2">
       <c r="A9" s="26" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="21" customFormat="1" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" s="21" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="24" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:2" s="24" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A11" s="25" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="26" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="21" customFormat="1" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" s="21" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="24" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:2" s="24" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A14" s="25" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="26" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="26" t="s">
         <v>34</v>
       </c>
@@ -4860,35 +4860,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d714a3296df14eba7a100bb665443ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49549bf45bfbbfb6cffed527380e77e1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5176,34 +5147,36 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F80F839-78EF-4FF4-A673-3CC84279C232}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5222,4 +5195,31 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
cronograma - fechamento juris_tcu
</commit_message>
<xml_diff>
--- a/docs/schedule/cronograma.xlsx
+++ b/docs/schedule/cronograma.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B2F0E3-8739-4959-971E-4704F1C6C855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B9D4B4-5774-4302-B737-79CFCB1E1CF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15870" yWindow="-6015" windowWidth="15990" windowHeight="24840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CronogramaDeProjeto" sheetId="11" r:id="rId1"/>
@@ -2113,26 +2113,25 @@
   </sheetPr>
   <dimension ref="A1:BD43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" sqref="I1:AP1048576"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7265625" style="31" customWidth="1"/>
+    <col min="1" max="1" width="2.77734375" style="31" customWidth="1"/>
     <col min="2" max="2" width="61" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" customWidth="1"/>
-    <col min="4" max="4" width="10.7265625" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="10.453125" customWidth="1"/>
-    <col min="7" max="7" width="2.7265625" customWidth="1"/>
-    <col min="8" max="8" width="6.26953125" hidden="1" customWidth="1"/>
-    <col min="9" max="42" width="2.54296875" hidden="1" customWidth="1"/>
-    <col min="43" max="51" width="2.54296875" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" customWidth="1"/>
+    <col min="7" max="7" width="2.77734375" customWidth="1"/>
+    <col min="8" max="8" width="6.21875" customWidth="1"/>
+    <col min="9" max="51" width="2.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" ht="26.25" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:56" ht="26.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
@@ -2145,7 +2144,7 @@
       <c r="F1" s="20"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:56" ht="24.75" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:56" ht="24.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="32"/>
       <c r="B2" s="92" t="s">
         <v>73</v>
@@ -2156,7 +2155,7 @@
       <c r="F2" s="20"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="31" t="s">
         <v>1</v>
       </c>
@@ -2171,7 +2170,7 @@
       </c>
       <c r="BD3" s="100"/>
     </row>
-    <row r="4" spans="1:56" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:56" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="31" t="s">
         <v>2</v>
       </c>
@@ -2185,7 +2184,7 @@
       </c>
       <c r="F4" s="106"/>
     </row>
-    <row r="5" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="32" t="s">
         <v>3</v>
       </c>
@@ -2248,7 +2247,7 @@
       <c r="AX5" s="104"/>
       <c r="AY5" s="54"/>
     </row>
-    <row r="6" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="32" t="s">
         <v>4</v>
       </c>
@@ -2431,7 +2430,7 @@
         <v>45106</v>
       </c>
     </row>
-    <row r="7" spans="1:56" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:56" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="32" t="s">
         <v>5</v>
       </c>
@@ -2627,7 +2626,7 @@
         <v>q</v>
       </c>
     </row>
-    <row r="8" spans="1:56" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:56" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="31" t="s">
         <v>6</v>
       </c>
@@ -2681,7 +2680,7 @@
       <c r="AX8" s="18"/>
       <c r="AY8" s="18"/>
     </row>
-    <row r="9" spans="1:56" s="2" customFormat="1" ht="18.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:56" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="32" t="s">
         <v>7</v>
       </c>
@@ -2741,7 +2740,7 @@
       <c r="AX9" s="18"/>
       <c r="AY9" s="57"/>
     </row>
-    <row r="10" spans="1:56" s="2" customFormat="1" ht="18.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:56" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="32" t="s">
         <v>8</v>
       </c>
@@ -2810,7 +2809,7 @@
       <c r="AX10" s="18"/>
       <c r="AY10" s="57"/>
     </row>
-    <row r="11" spans="1:56" s="2" customFormat="1" ht="18.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:56" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="32" t="s">
         <v>9</v>
       </c>
@@ -2878,7 +2877,7 @@
       <c r="AX11" s="18"/>
       <c r="AY11" s="57"/>
     </row>
-    <row r="12" spans="1:56" s="2" customFormat="1" ht="18.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:56" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="31"/>
       <c r="B12" s="40" t="s">
         <v>37</v>
@@ -2945,7 +2944,7 @@
       <c r="AY12" s="57"/>
       <c r="BD12" s="99"/>
     </row>
-    <row r="13" spans="1:56" s="2" customFormat="1" ht="18.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:56" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="31"/>
       <c r="B13" s="40" t="s">
         <v>38</v>
@@ -3011,7 +3010,7 @@
       <c r="AX13" s="18"/>
       <c r="AY13" s="57"/>
     </row>
-    <row r="14" spans="1:56" s="2" customFormat="1" ht="18.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:56" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="32" t="s">
         <v>55</v>
       </c>
@@ -3071,7 +3070,7 @@
       <c r="AX14" s="18"/>
       <c r="AY14" s="57"/>
     </row>
-    <row r="15" spans="1:56" s="2" customFormat="1" ht="18.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:56" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="32" t="s">
         <v>55</v>
       </c>
@@ -3139,7 +3138,7 @@
       <c r="AX15" s="18"/>
       <c r="AY15" s="57"/>
     </row>
-    <row r="16" spans="1:56" s="2" customFormat="1" ht="18.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:56" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="32" t="s">
         <v>55</v>
       </c>
@@ -3207,7 +3206,7 @@
       <c r="AX16" s="18"/>
       <c r="AY16" s="57"/>
     </row>
-    <row r="17" spans="1:51" s="2" customFormat="1" ht="18.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="32" t="s">
         <v>55</v>
       </c>
@@ -3275,7 +3274,7 @@
       <c r="AX17" s="18"/>
       <c r="AY17" s="57"/>
     </row>
-    <row r="18" spans="1:51" s="2" customFormat="1" ht="18.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="31"/>
       <c r="B18" s="74" t="s">
         <v>59</v>
@@ -3341,7 +3340,7 @@
       <c r="AX18" s="18"/>
       <c r="AY18" s="57"/>
     </row>
-    <row r="19" spans="1:51" s="2" customFormat="1" ht="18.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="32" t="s">
         <v>55</v>
       </c>
@@ -3409,7 +3408,7 @@
       <c r="AX19" s="18"/>
       <c r="AY19" s="57"/>
     </row>
-    <row r="20" spans="1:51" s="2" customFormat="1" ht="18.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="31"/>
       <c r="B20" s="76" t="s">
         <v>58</v>
@@ -3475,7 +3474,7 @@
       <c r="AX20" s="18"/>
       <c r="AY20" s="57"/>
     </row>
-    <row r="21" spans="1:51" s="2" customFormat="1" ht="18.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="32" t="s">
         <v>55</v>
       </c>
@@ -3535,7 +3534,7 @@
       <c r="AX21" s="18"/>
       <c r="AY21" s="57"/>
     </row>
-    <row r="22" spans="1:51" s="2" customFormat="1" ht="18.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="31"/>
       <c r="B22" s="41" t="s">
         <v>67</v>
@@ -3601,7 +3600,7 @@
       <c r="AX22" s="18"/>
       <c r="AY22" s="57"/>
     </row>
-    <row r="23" spans="1:51" s="2" customFormat="1" ht="18.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="31"/>
       <c r="B23" s="41" t="s">
         <v>41</v>
@@ -3667,7 +3666,7 @@
       <c r="AX23" s="18"/>
       <c r="AY23" s="57"/>
     </row>
-    <row r="24" spans="1:51" s="2" customFormat="1" ht="18.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="31"/>
       <c r="B24" s="41" t="s">
         <v>61</v>
@@ -3676,7 +3675,7 @@
         <v>39</v>
       </c>
       <c r="D24" s="16">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E24" s="50">
         <v>45092</v>
@@ -3733,7 +3732,7 @@
       <c r="AX24" s="18"/>
       <c r="AY24" s="57"/>
     </row>
-    <row r="25" spans="1:51" s="2" customFormat="1" ht="18.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="31"/>
       <c r="B25" s="41" t="s">
         <v>52</v>
@@ -3742,7 +3741,7 @@
         <v>50</v>
       </c>
       <c r="D25" s="16">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="E25" s="50">
         <v>45093</v>
@@ -3799,7 +3798,7 @@
       <c r="AX25" s="18"/>
       <c r="AY25" s="57"/>
     </row>
-    <row r="26" spans="1:51" s="2" customFormat="1" ht="18.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="32" t="s">
         <v>10</v>
       </c>
@@ -3859,7 +3858,7 @@
       <c r="AX26" s="18"/>
       <c r="AY26" s="57"/>
     </row>
-    <row r="27" spans="1:51" s="2" customFormat="1" ht="18.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="32"/>
       <c r="B27" s="81" t="s">
         <v>63</v>
@@ -3925,7 +3924,7 @@
       <c r="AX27" s="18"/>
       <c r="AY27" s="57"/>
     </row>
-    <row r="28" spans="1:51" s="2" customFormat="1" ht="18.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="31"/>
       <c r="B28" s="79" t="s">
         <v>64</v>
@@ -3991,7 +3990,7 @@
       <c r="AX28" s="18"/>
       <c r="AY28" s="57"/>
     </row>
-    <row r="29" spans="1:51" s="2" customFormat="1" ht="18.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="32"/>
       <c r="B29" s="81" t="s">
         <v>65</v>
@@ -4057,7 +4056,7 @@
       <c r="AX29" s="18"/>
       <c r="AY29" s="57"/>
     </row>
-    <row r="30" spans="1:51" s="2" customFormat="1" ht="18.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="31"/>
       <c r="B30" s="79" t="s">
         <v>40</v>
@@ -4123,7 +4122,7 @@
       <c r="AX30" s="18"/>
       <c r="AY30" s="57"/>
     </row>
-    <row r="31" spans="1:51" s="2" customFormat="1" ht="18.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="31"/>
       <c r="B31" s="79" t="s">
         <v>78</v>
@@ -4189,7 +4188,7 @@
       <c r="AX31" s="18"/>
       <c r="AY31" s="57"/>
     </row>
-    <row r="32" spans="1:51" s="2" customFormat="1" ht="18.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="32" t="s">
         <v>10</v>
       </c>
@@ -4249,7 +4248,7 @@
       <c r="AX32" s="18"/>
       <c r="AY32" s="57"/>
     </row>
-    <row r="33" spans="1:51" s="2" customFormat="1" ht="18.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="32"/>
       <c r="B33" s="74" t="s">
         <v>63</v>
@@ -4315,7 +4314,7 @@
       <c r="AX33" s="18"/>
       <c r="AY33" s="57"/>
     </row>
-    <row r="34" spans="1:51" s="2" customFormat="1" ht="18.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="31"/>
       <c r="B34" s="76" t="s">
         <v>64</v>
@@ -4381,7 +4380,7 @@
       <c r="AX34" s="18"/>
       <c r="AY34" s="57"/>
     </row>
-    <row r="35" spans="1:51" s="2" customFormat="1" ht="18.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="31"/>
       <c r="B35" s="76" t="s">
         <v>79</v>
@@ -4447,7 +4446,7 @@
       <c r="AX35" s="18"/>
       <c r="AY35" s="57"/>
     </row>
-    <row r="36" spans="1:51" s="2" customFormat="1" ht="18.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="31" t="s">
         <v>11</v>
       </c>
@@ -4507,7 +4506,7 @@
       <c r="AX36" s="18"/>
       <c r="AY36" s="57"/>
     </row>
-    <row r="37" spans="1:51" s="2" customFormat="1" ht="18.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="31"/>
       <c r="B37" s="41" t="s">
         <v>42</v>
@@ -4573,7 +4572,7 @@
       <c r="AX37" s="18"/>
       <c r="AY37" s="57"/>
     </row>
-    <row r="38" spans="1:51" s="2" customFormat="1" ht="18.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="31"/>
       <c r="B38" s="93" t="s">
         <v>66</v>
@@ -4588,12 +4587,12 @@
         <v>45101</v>
       </c>
       <c r="F38" s="50">
-        <v>45107</v>
+        <v>45105</v>
       </c>
       <c r="G38" s="59"/>
       <c r="H38" s="59">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I38" s="60"/>
       <c r="J38" s="60"/>
@@ -4639,7 +4638,7 @@
       <c r="AX38" s="60"/>
       <c r="AY38" s="61"/>
     </row>
-    <row r="39" spans="1:51" s="2" customFormat="1" ht="18.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:51" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="31"/>
       <c r="B39" s="93" t="s">
         <v>69</v>
@@ -4648,7 +4647,7 @@
         <v>39</v>
       </c>
       <c r="D39" s="95">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="E39" s="96">
         <v>45081</v>
@@ -4705,7 +4704,7 @@
       <c r="AX39" s="60"/>
       <c r="AY39" s="61"/>
     </row>
-    <row r="40" spans="1:51" s="65" customFormat="1" ht="22.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:51" s="65" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="66" t="s">
         <v>12</v>
       </c>
@@ -4722,16 +4721,16 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:51" s="71" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:51" s="71" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="62"/>
       <c r="E41" s="72"/>
       <c r="G41" s="73"/>
     </row>
-    <row r="42" spans="1:51" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:51" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C42" s="8"/>
       <c r="F42" s="33"/>
     </row>
-    <row r="43" spans="1:51" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:51" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C43" s="9"/>
     </row>
   </sheetData>
@@ -4832,31 +4831,31 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="94.453125" style="21" customWidth="1"/>
-    <col min="2" max="16384" width="9.26953125" style="1"/>
+    <col min="1" max="1" width="94.44140625" style="21" customWidth="1"/>
+    <col min="2" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:2" s="23" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="22"/>
     </row>
-    <row r="3" spans="1:2" s="27" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" s="27" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="44" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="28"/>
     </row>
-    <row r="4" spans="1:2" s="24" customFormat="1" ht="26" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:2" s="24" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A4" s="25" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
         <v>23</v>
       </c>
@@ -4866,42 +4865,42 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="21" customFormat="1" ht="205.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" s="21" customFormat="1" ht="205.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="30" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="24" customFormat="1" ht="26" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:2" s="24" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A8" s="25" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="58" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="26" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="21" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" s="21" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="24" customFormat="1" ht="26" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:2" s="24" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A11" s="25" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="29" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="26" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="21" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" s="21" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="29" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="24" customFormat="1" ht="26" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:2" s="24" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A14" s="25" t="s">
         <v>32</v>
       </c>
@@ -4930,35 +4929,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d714a3296df14eba7a100bb665443ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49549bf45bfbbfb6cffed527380e77e1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5246,34 +5216,36 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F80F839-78EF-4FF4-A673-3CC84279C232}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5292,4 +5264,31 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>